<commit_message>
changes the excel files
</commit_message>
<xml_diff>
--- a/webrouting/Documents/Program Documents/Contacts - SAMPLE.xlsx
+++ b/webrouting/Documents/Program Documents/Contacts - SAMPLE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CPSC 488 Software Engineering\excel samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dakot\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB6577B-E968-4E31-833B-0D9406B47DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC6DF9F-C7F7-400A-81AD-AE74A3EAB4E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{6F7B2A25-9F4D-490E-B70D-6C9AB6577A80}"/>
+    <workbookView xWindow="7545" yWindow="3720" windowWidth="27045" windowHeight="15195" xr2:uid="{6F7B2A25-9F4D-490E-B70D-6C9AB6577A80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,18 +71,9 @@
     <t>Work Phone</t>
   </si>
   <si>
-    <t>Dakota</t>
-  </si>
-  <si>
-    <t>Myers</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
-    <t>drm1022@sru.edu</t>
-  </si>
-  <si>
     <t>5 Wallaby Street</t>
   </si>
   <si>
@@ -288,6 +279,15 @@
   </si>
   <si>
     <t>Room 2</t>
+  </si>
+  <si>
+    <t>Franz</t>
+  </si>
+  <si>
+    <t>Ferdinand</t>
+  </si>
+  <si>
+    <t>therockband@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -735,7 +735,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,316 +794,315 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="D2" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="I2" s="7">
         <v>16057</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I3" s="7">
         <v>90210</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="F4" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="I4" s="7">
         <v>43140</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I5" s="7">
         <v>16323</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="F6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>48</v>
-      </c>
       <c r="H6" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I6" s="7">
         <v>15106</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="F7" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>55</v>
-      </c>
       <c r="H7" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I7" s="7">
         <v>16117</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="E8" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I8" s="7">
         <v>15204</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="F9" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="H9" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>68</v>
       </c>
       <c r="I9" s="7">
         <v>21201</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="F10" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="H10" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="I10" s="7">
         <v>2116</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{53F3858D-E2FB-49FF-A6AD-8B7F3E390C7B}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{86BB99D8-338D-4851-A373-CE42134B575E}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{14344E1D-DFB4-44D9-A6B3-D5F935E42AD9}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{7835534C-348E-4727-9A97-1D3AD3C89624}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{DE246F06-3986-44B7-9FA4-268DA905EE2C}"/>
-    <hyperlink ref="D8" r:id="rId6" xr:uid="{2BE0A223-E2FE-44C1-B586-016239D2DF82}"/>
-    <hyperlink ref="D7" r:id="rId7" xr:uid="{21285CF2-9464-4207-ADF0-0A1A077C9EFD}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{1532AF6D-6272-47D0-9F47-D5153B620448}"/>
-    <hyperlink ref="D10" r:id="rId9" xr:uid="{A6BCC042-A0D8-47BE-B32C-1885093B4F42}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{86BB99D8-338D-4851-A373-CE42134B575E}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{14344E1D-DFB4-44D9-A6B3-D5F935E42AD9}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{7835534C-348E-4727-9A97-1D3AD3C89624}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{DE246F06-3986-44B7-9FA4-268DA905EE2C}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{2BE0A223-E2FE-44C1-B586-016239D2DF82}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{21285CF2-9464-4207-ADF0-0A1A077C9EFD}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{1532AF6D-6272-47D0-9F47-D5153B620448}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{A6BCC042-A0D8-47BE-B32C-1885093B4F42}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>